<commit_message>
Fixed date bug with american/british times in result combiner
</commit_message>
<xml_diff>
--- a/ResultCombiner/ResultCombiner/bin/Debug/Users/Peter Lockhart.xlsx
+++ b/ResultCombiner/ResultCombiner/bin/Debug/Users/Peter Lockhart.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\GitHub\CSC4001\ResultCombiner\ResultCombiner\bin\Debug\Users\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b36e309a77704392/Documents/CSC 4001/ExperimentResults/Users/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="9990" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="9990"/>
   </bookViews>
   <sheets>
     <sheet name="Exp 3" sheetId="5" r:id="rId1"/>
@@ -404,9 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -428,14 +426,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2">
-        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -832,9 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -856,14 +846,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>43</v>
-      </c>
       <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2">
-        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -1550,9 +1534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1574,14 +1556,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>134</v>
-      </c>
       <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2">
-        <v>134</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -3566,9 +3542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3590,14 +3564,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>42</v>
-      </c>
       <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2">
-        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -4282,9 +4250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>